<commit_message>
V1 primera carga basica
</commit_message>
<xml_diff>
--- a/GPIO_Teclado_Macros_V1.xlsx
+++ b/GPIO_Teclado_Macros_V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositorios\Proyectos Finalizados\Teclado Macro BT ESP32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\Proyectos 2024\Teclado-Macros-BT-ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F3EB42-5A3E-4F05-AF71-01684EE05471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FAD1774-7452-4405-809E-6DC76023462E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1CC31A59-071C-4B79-B480-A3CD3D0586A2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1CC31A59-071C-4B79-B480-A3CD3D0586A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>GPIO</t>
   </si>
@@ -80,18 +80,12 @@
     <t>Page Down</t>
   </si>
   <si>
-    <t>Page Up</t>
-  </si>
-  <si>
     <t>Ctrl + Alt + Shift + F5</t>
   </si>
   <si>
     <t>Ctrl + Alt + Shift + F6</t>
   </si>
   <si>
-    <t>PrintScreen o win shift s</t>
-  </si>
-  <si>
     <t>Ctrl + Alt + Shift + F7</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>S15</t>
   </si>
   <si>
-    <t>D7</t>
-  </si>
-  <si>
     <t>D19</t>
   </si>
   <si>
@@ -162,6 +153,39 @@
   </si>
   <si>
     <t>D14</t>
+  </si>
+  <si>
+    <t>D21</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>D33</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + Shift + F8</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + Shift + F9</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + Shift + F10</t>
+  </si>
+  <si>
+    <t>CTR C</t>
+  </si>
+  <si>
+    <t>CTR V</t>
+  </si>
+  <si>
+    <t>CTR Z</t>
+  </si>
+  <si>
+    <t>Page UP</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + Shift + F11</t>
   </si>
 </sst>
 </file>
@@ -582,28 +606,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D00BFD8-8064-4ED2-A3E0-704A30F9AE96}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:E12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="4"/>
+    <col min="1" max="16384" width="11.44140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -612,21 +638,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -634,18 +660,18 @@
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>4</v>
@@ -654,49 +680,49 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>7</v>
       </c>
@@ -704,119 +730,119 @@
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
SW EspHome para incluir como dispositivo a Home Assistant y comienzo de version multiperfil
</commit_message>
<xml_diff>
--- a/GPIO_Teclado_Macros_V1.xlsx
+++ b/GPIO_Teclado_Macros_V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\Proyectos 2024\Teclado-Macros-BT-ESP32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositorios\Proyectos Finalizados\Teclado-Macros-BT-ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FAD1774-7452-4405-809E-6DC76023462E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06A4D84-2EF9-49D0-A2B7-2CF67F8AE6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1CC31A59-071C-4B79-B480-A3CD3D0586A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1CC31A59-071C-4B79-B480-A3CD3D0586A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
   <si>
     <t>GPIO</t>
   </si>
@@ -186,6 +186,111 @@
   </si>
   <si>
     <t>Ctrl + Alt + Shift + F11</t>
+  </si>
+  <si>
+    <t>CTR+c</t>
+  </si>
+  <si>
+    <t>CTR+v</t>
+  </si>
+  <si>
+    <t>CTR+z</t>
+  </si>
+  <si>
+    <t>Profile Down</t>
+  </si>
+  <si>
+    <t>Profile UP</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F2</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F3</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F4</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F5</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F6</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F7</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F8</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F9</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F10</t>
+  </si>
+  <si>
+    <t>ALT+ CTR+ SHIFT+ F11</t>
+  </si>
+  <si>
+    <t>CTR+ F7</t>
+  </si>
+  <si>
+    <t>SHIFT+ F7</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>Perfil 2 (Automation Builder)</t>
+  </si>
+  <si>
+    <t>Perfil 1 (Standar)</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15</t>
   </si>
 </sst>
 </file>
@@ -215,7 +320,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,19 +367,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,18 +718,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D00BFD8-8064-4ED2-A3E0-704A30F9AE96}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.44140625" style="4"/>
+    <col min="1" max="6" width="11.42578125" style="4"/>
+    <col min="7" max="7" width="13.5703125" style="4" customWidth="1"/>
+    <col min="8" max="10" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -624,7 +743,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -638,210 +757,351 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="3">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="3">
+      <c r="H3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="3">
+      <c r="H4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="3">
+      <c r="H5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="3">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
+      <c r="G7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="3">
+      <c r="H8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="3">
+      <c r="H9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
+      <c r="G11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
+      <c r="H12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
+      <c r="H13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="1" t="s">

</xml_diff>